<commit_message>
Added load cell + amplifier from DEBO
</commit_message>
<xml_diff>
--- a/B.0 System Design/SAN_Project_Partslist.xlsx
+++ b/B.0 System Design/SAN_Project_Partslist.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Projects\LoRaProject\B.0 System Design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2ad1c0a53281c2ab/Documents/University/Studies/Sem 5/Sensors and Actuator Networks/Project/B.0 System Design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B84344F-A1E2-4550-9753-47CC572F610C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{4B84344F-A1E2-4550-9753-47CC572F610C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9A71D272-D835-40C4-9F5D-FC7C440C1AE3}"/>
   <workbookProtection lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts" sheetId="5" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="80">
   <si>
     <t>Link</t>
   </si>
@@ -262,6 +262,18 @@
   </si>
   <si>
     <t>Microchip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Load cell + amplifier </t>
+  </si>
+  <si>
+    <t>DEBO HX711-01</t>
+  </si>
+  <si>
+    <t>SEN-HX711-01</t>
+  </si>
+  <si>
+    <t>https://www.reichelt.com/de/en/shop/product/developer_boards_-_a_d_converter_-_balance-316296#closemodal</t>
   </si>
 </sst>
 </file>
@@ -654,6 +666,49 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -667,49 +722,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1018,62 +1030,62 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
-    <col min="2" max="2" width="4.88671875" customWidth="1"/>
-    <col min="3" max="3" width="12.44140625" customWidth="1"/>
-    <col min="4" max="4" width="14.44140625" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" customWidth="1"/>
-    <col min="6" max="6" width="7.6640625" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" customWidth="1"/>
-    <col min="8" max="8" width="8.6640625" customWidth="1"/>
-    <col min="9" max="9" width="6.5546875" customWidth="1"/>
-    <col min="10" max="10" width="55.33203125" customWidth="1"/>
-    <col min="13" max="13" width="12.33203125" customWidth="1"/>
-    <col min="20" max="20" width="9.44140625" customWidth="1"/>
-    <col min="21" max="21" width="17.6640625" customWidth="1"/>
+    <col min="2" max="2" width="4.85546875" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" customWidth="1"/>
+    <col min="9" max="9" width="6.5703125" customWidth="1"/>
+    <col min="10" max="10" width="55.28515625" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" customWidth="1"/>
+    <col min="20" max="20" width="9.42578125" customWidth="1"/>
+    <col min="21" max="21" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="49" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="50"/>
+      <c r="B1" s="55"/>
       <c r="C1" s="20" t="s">
         <v>23</v>
       </c>
       <c r="G1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="45" t="s">
+      <c r="H1" s="59" t="s">
         <v>39</v>
       </c>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="49" t="s">
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="50"/>
+      <c r="B2" s="55"/>
       <c r="C2" s="21" t="s">
         <v>40</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="46" t="s">
+      <c r="H2" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-    </row>
-    <row r="4" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="I2" s="60"/>
+      <c r="J2" s="60"/>
+    </row>
+    <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
@@ -1105,7 +1117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="46.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>1</v>
       </c>
@@ -1138,7 +1150,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>2</v>
       </c>
@@ -1171,7 +1183,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>3</v>
       </c>
@@ -1204,7 +1216,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>4</v>
       </c>
@@ -1237,7 +1249,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>5</v>
       </c>
@@ -1256,7 +1268,7 @@
       <c r="F9" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="G9" s="62" t="s">
+      <c r="G9" s="45" t="s">
         <v>60</v>
       </c>
       <c r="H9" s="28">
@@ -1270,7 +1282,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>6</v>
       </c>
@@ -1303,7 +1315,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>7</v>
       </c>
@@ -1336,7 +1348,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>8</v>
       </c>
@@ -1369,24 +1381,40 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>9</v>
       </c>
-      <c r="B13" s="29"/>
-      <c r="C13" s="30"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="31"/>
+      <c r="B13" s="29">
+        <v>1</v>
+      </c>
+      <c r="C13" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="E13" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="F13" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="H13" s="31">
+        <v>6.4</v>
+      </c>
       <c r="I13" s="31">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J13" s="38"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+        <v>6.4</v>
+      </c>
+      <c r="J13" s="38" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>10</v>
       </c>
@@ -1403,7 +1431,7 @@
       </c>
       <c r="J14" s="38"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>11</v>
       </c>
@@ -1420,7 +1448,7 @@
       </c>
       <c r="J15" s="38"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>12</v>
       </c>
@@ -1437,7 +1465,7 @@
       </c>
       <c r="J16" s="38"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <v>13</v>
       </c>
@@ -1454,7 +1482,7 @@
       </c>
       <c r="J17" s="38"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
         <v>14</v>
       </c>
@@ -1471,7 +1499,7 @@
       </c>
       <c r="J18" s="38"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
         <v>15</v>
       </c>
@@ -1488,18 +1516,18 @@
       </c>
       <c r="J19" s="39"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="G20" s="47" t="s">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G20" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="H20" s="47"/>
+      <c r="H20" s="61"/>
       <c r="I20" s="13">
         <f>SUM(I5:I19)</f>
-        <v>48.6</v>
+        <v>55</v>
       </c>
       <c r="J20" s="4"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
         <v>25</v>
       </c>
@@ -1507,103 +1535,103 @@
       <c r="C21" s="15"/>
       <c r="D21" s="15"/>
       <c r="E21" s="16"/>
-      <c r="G21" s="48" t="s">
+      <c r="G21" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="H21" s="48"/>
+      <c r="H21" s="62"/>
       <c r="I21" s="11">
         <f>I20*0.19</f>
-        <v>9.234</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" s="51" t="s">
+        <v>10.45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="52"/>
+      <c r="B22" s="57"/>
       <c r="C22" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="D22" s="52" t="s">
+      <c r="D22" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="E22" s="55"/>
-      <c r="G22" s="48" t="s">
+      <c r="E22" s="58"/>
+      <c r="G22" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="H22" s="48"/>
+      <c r="H22" s="62"/>
       <c r="I22" s="12">
         <f>I20*1.19</f>
-        <v>57.833999999999996</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23" s="53" t="s">
+        <v>65.45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="54"/>
+      <c r="B23" s="47"/>
       <c r="C23" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D23" s="58" t="s">
+      <c r="D23" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="E23" s="59"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" s="53" t="s">
+      <c r="E23" s="51"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="B24" s="54"/>
+      <c r="B24" s="47"/>
       <c r="C24" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="D24" s="58" t="s">
+      <c r="D24" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="E24" s="59"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25" s="53" t="s">
+      <c r="E24" s="51"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="B25" s="54"/>
+      <c r="B25" s="47"/>
       <c r="C25" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="58" t="s">
+      <c r="D25" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E25" s="59"/>
+      <c r="E25" s="51"/>
       <c r="H25" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A26" s="53" t="s">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="54"/>
+      <c r="B26" s="47"/>
       <c r="C26" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="D26" s="58" t="s">
+      <c r="D26" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="E26" s="59"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A27" s="56" t="s">
+      <c r="E26" s="51"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="57"/>
+      <c r="B27" s="49"/>
       <c r="C27" s="40"/>
-      <c r="D27" s="60" t="s">
+      <c r="D27" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="E27" s="61"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E27" s="53"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="41" t="s">
         <v>55</v>
       </c>
@@ -1616,7 +1644,7 @@
       </c>
       <c r="E28" s="43"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="1"/>
@@ -1628,7 +1656,7 @@
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="2"/>
@@ -1640,7 +1668,7 @@
       <c r="I43" s="1"/>
       <c r="J43" s="3"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="2"/>
@@ -1652,7 +1680,7 @@
       <c r="I44" s="1"/>
       <c r="J44" s="3"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="2"/>
@@ -1664,7 +1692,7 @@
       <c r="I45" s="1"/>
       <c r="J45" s="3"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="2"/>
@@ -1676,7 +1704,7 @@
       <c r="I46" s="1"/>
       <c r="J46" s="3"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -1688,7 +1716,7 @@
       <c r="I47" s="1"/>
       <c r="J47" s="3"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="2"/>
@@ -1700,7 +1728,7 @@
       <c r="I48" s="1"/>
       <c r="J48" s="3"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="2"/>
@@ -1714,6 +1742,16 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="D22:E22"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="A27:B27"/>
@@ -1723,16 +1761,6 @@
     <mergeCell ref="D27:E27"/>
     <mergeCell ref="A26:B26"/>
     <mergeCell ref="D26:E26"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="G22:H22"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F19" xr:uid="{00000000-0002-0000-0000-000000000000}">
@@ -1748,9 +1776,11 @@
     <hyperlink ref="D28" r:id="rId6" xr:uid="{82C4D3B1-9958-460D-9331-581AF47D3A7F}"/>
     <hyperlink ref="J8" r:id="rId7" location="closemodal" xr:uid="{0BC7397E-CC1B-49DB-89D0-5C72D081FAD8}"/>
     <hyperlink ref="J9" r:id="rId8" xr:uid="{E91E3A8F-2A46-42AE-9608-F60A317835D9}"/>
+    <hyperlink ref="J5" r:id="rId9" xr:uid="{BABD9659-74D3-459A-97A1-C25E7F0C18FA}"/>
+    <hyperlink ref="J6" r:id="rId10" xr:uid="{8B82B98C-F63E-43A1-AE2D-80461502EDCE}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" r:id="rId9"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId11"/>
   <headerFooter>
     <oddHeader>&amp;CParts list
 Sensors and Actuator Networks</oddHeader>

</xml_diff>